<commit_message>
Working on the design class
</commit_message>
<xml_diff>
--- a/exampleRateData.xlsx
+++ b/exampleRateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e5d38b718110f79/Documents/GitHub/CorrelationAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{1233D6C7-3FE8-4C3C-A216-AC950F8A747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F0AE1E8-BF4C-4E25-910A-379BF4DA0B99}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{1233D6C7-3FE8-4C3C-A216-AC950F8A747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{873CE856-595E-480D-B316-5142A02AEC2B}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09C01337-4956-4B76-99F7-501478173D17}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>[Deg C]</t>
   </si>
   <si>
-    <t>C-Rate</t>
-  </si>
-  <si>
     <t>LGM50</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>BatteryName</t>
+  </si>
+  <si>
+    <t>CRate</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -471,13 +471,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -489,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -517,7 +517,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>11</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>11</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>11</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>11</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>12</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31">
         <v>12</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32">
         <v>12</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33">
         <v>13</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>13</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35">
         <v>13</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36">
         <v>13</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37">
         <v>13</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38">
         <v>14</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39">
         <v>14</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40">
         <v>14</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41">
         <v>14</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42">
         <v>14</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>16</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44">
         <v>16</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45">
         <v>16</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46">
         <v>16</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47">
         <v>16</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B59">
         <v>8</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65">
         <v>10</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66">
         <v>10</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B67">
         <v>10</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B68">
         <v>13</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B69">
         <v>13</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B70">
         <v>13</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B71">
         <v>13</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B72">
         <v>13</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B73">
         <v>14</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B74">
         <v>14</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B75">
         <v>14</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B76">
         <v>14</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B77">
         <v>14</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B83">
         <v>18</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B84">
         <v>18</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B85">
         <v>18</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B86">
         <v>18</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B87">
         <v>18</v>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B88">
         <v>19</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B89">
         <v>19</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B90">
         <v>19</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B91">
         <v>19</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B92">
         <v>19</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B93">
         <v>781</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94">
         <v>781</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B95">
         <v>781</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B96">
         <v>781</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B97">
         <v>781</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B98">
         <v>782</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B99">
         <v>782</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B100">
         <v>782</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B101">
         <v>782</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B102">
         <v>782</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B103">
         <v>783</v>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B104">
         <v>783</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B105">
         <v>783</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B106">
         <v>783</v>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B107">
         <v>783</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B108">
         <v>784</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B109">
         <v>784</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B110">
         <v>784</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B111">
         <v>784</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B112">
         <v>784</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B113">
         <v>785</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B114">
         <v>785</v>
@@ -3093,7 +3093,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B115">
         <v>785</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B116">
         <v>785</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B117">
         <v>785</v>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B118">
         <v>786</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B119">
         <v>786</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B120">
         <v>786</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B121">
         <v>786</v>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B122">
         <v>786</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B123">
         <v>787</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B124">
         <v>787</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B125">
         <v>787</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B126">
         <v>787</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B127">
         <v>787</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B128">
         <v>788</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B129">
         <v>788</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B130">
         <v>788</v>
@@ -3461,7 +3461,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B131">
         <v>788</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B132">
         <v>788</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B133">
         <v>789</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B134">
         <v>789</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B135">
         <v>789</v>
@@ -3576,7 +3576,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B136">
         <v>789</v>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B137">
         <v>789</v>
@@ -3622,7 +3622,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B138">
         <v>790</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B139">
         <v>790</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B140">
         <v>790</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B141">
         <v>790</v>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B142">
         <v>790</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B143">
         <v>791</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B144">
         <v>791</v>
@@ -3783,7 +3783,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B145">
         <v>791</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B146">
         <v>791</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B147">
         <v>791</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B148">
         <v>792</v>
@@ -3875,7 +3875,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B149">
         <v>792</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B150">
         <v>792</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B151">
         <v>792</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B152">
         <v>792</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B153">
         <v>793</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B154">
         <v>793</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B155">
         <v>793</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B156">
         <v>793</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B157">
         <v>793</v>
@@ -4082,7 +4082,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B158">
         <v>794</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B159">
         <v>794</v>
@@ -4128,7 +4128,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B160">
         <v>794</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B161">
         <v>794</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B162">
         <v>794</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B163">
         <v>795</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B164">
         <v>795</v>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B165">
         <v>795</v>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B166">
         <v>795</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B167">
         <v>795</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B168">
         <v>796</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B169">
         <v>796</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B170">
         <v>796</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B171">
         <v>796</v>
@@ -4404,7 +4404,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B172">
         <v>796</v>
@@ -4427,7 +4427,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B173">
         <v>797</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B174">
         <v>797</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B175">
         <v>797</v>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B176">
         <v>797</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B177">
         <v>797</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B178">
         <v>798</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B179">
         <v>798</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B180">
         <v>798</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B181">
         <v>798</v>
@@ -4634,7 +4634,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B182">
         <v>798</v>

</xml_diff>